<commit_message>
AIE/F/14-IIR: Updated for 2023.1
</commit_message>
<xml_diff>
--- a/AI_Engine_Development/Feature_Tutorials/14-implementing-iir-filter/Part2b/api_thruput.xlsx
+++ b/AI_Engine_Development/Feature_Tutorials/14-implementing-iir-filter/Part2b/api_thruput.xlsx
@@ -37,7 +37,7 @@
     <t xml:space="preserve">num_cycles (API)</t>
   </si>
   <si>
-    <t xml:space="preserve">API Throughput (Msa/sec))</t>
+    <t xml:space="preserve">API Throughput (Msa/sec)</t>
   </si>
 </sst>
 </file>
@@ -164,10 +164,10 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A14" activeCellId="0" sqref="A14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.51"/>
   </cols>
@@ -249,25 +249,25 @@
         <v>4</v>
       </c>
       <c r="B7" s="0" t="n">
-        <v>289</v>
+        <v>187</v>
       </c>
       <c r="C7" s="0" t="n">
-        <v>799</v>
+        <v>492</v>
       </c>
       <c r="D7" s="0" t="n">
-        <v>1508</v>
+        <v>940</v>
       </c>
       <c r="E7" s="0" t="n">
-        <v>2925</v>
+        <v>1836</v>
       </c>
       <c r="F7" s="0" t="n">
-        <v>5761</v>
+        <v>3628</v>
       </c>
       <c r="G7" s="0" t="n">
-        <v>11431</v>
+        <v>7212</v>
       </c>
       <c r="H7" s="0" t="n">
-        <v>22772</v>
+        <v>14379</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -276,31 +276,31 @@
       </c>
       <c r="B9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*B6/B7</f>
-        <v>27.681660899654</v>
+        <v>42.7807486631016</v>
       </c>
       <c r="C9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*C6/C7</f>
-        <v>80.1001251564456</v>
+        <v>130.081300813008</v>
       </c>
       <c r="D9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*D6/D7</f>
-        <v>84.8806366047745</v>
+        <v>136.170212765957</v>
       </c>
       <c r="E9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*E6/E7</f>
-        <v>87.5213675213675</v>
+        <v>139.433551198257</v>
       </c>
       <c r="F9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*F6/F7</f>
-        <v>88.8734594688422</v>
+        <v>141.124586549063</v>
       </c>
       <c r="G9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*G6/G7</f>
-        <v>89.5809640451404</v>
+        <v>141.985579589573</v>
       </c>
       <c r="H9" s="3" t="n">
         <f aca="false">0.000001*B3*1000000000*H6/H7</f>
-        <v>89.935007904444</v>
+        <v>142.42993254051</v>
       </c>
     </row>
   </sheetData>

</xml_diff>